<commit_message>
tests coverage and little fix
</commit_message>
<xml_diff>
--- a/tests/data/4_every_style.xlsx
+++ b/tests/data/4_every_style.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Development/xlnt/tests/data/"/>
     </mc:Choice>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>rotation 45</t>
+  </si>
+  <si>
+    <t>rows_groupping</t>
+  </si>
+  <si>
+    <t>collapsed</t>
+  </si>
+  <si>
+    <t>hidden, outline_level</t>
   </si>
 </sst>
 </file>
@@ -634,7 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="1" showOutlineSymbols="1"/>
+  </sheetPr>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
@@ -1135,6 +1147,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="36" spans="1:4" collapsed="1">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Outline level support (rows groupping) (#135)
To add row grouping functionality, the OutlineLevel parameter and
related settings were supported.

```
#include <contrib/libs/xlnt/include/xlnt/xlnt.hpp>
#include <iostream>

int main()
{
    xlnt::workbook wb;
    xlnt::worksheet ws = wb.active_sheet();

    // Create 4 rows, each on a new outline level
    for (int r = 1; r <= 4; ++r) {
        ws.cell(xlnt::cell_reference(1, r)).value("Level " + std::to_string(r - 1));

        auto props = ws.row_properties(r);
        props.outline_level = r - 1; // Levels 0, 1, 2, 3
        ws.add_row_properties(r, props);
    }

    // Configure outline settings
    ws.outline_settings(true, false, true, false);

    wb.save("outline_test.xlsx");
    std::cout << "Saved outline_test.xlsx" << std::endl;
    return 0;
}
```

This code will produce excel like this
<img width="210" height="152" alt="image"
src="https://github.com/user-attachments/assets/edeb83e4-dd36-4881-aa90-ddc017bbba2e"
/>
</commit_message>
<xml_diff>
--- a/tests/data/4_every_style.xlsx
+++ b/tests/data/4_every_style.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Development/xlnt/tests/data/"/>
     </mc:Choice>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>rotation 45</t>
+  </si>
+  <si>
+    <t>rows_groupping</t>
+  </si>
+  <si>
+    <t>collapsed</t>
+  </si>
+  <si>
+    <t>hidden, outline_level</t>
   </si>
 </sst>
 </file>
@@ -634,7 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="1" showOutlineSymbols="1"/>
+  </sheetPr>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
@@ -1135,6 +1147,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="36" spans="1:4" collapsed="1">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>